<commit_message>
added parallel and single run features
</commit_message>
<xml_diff>
--- a/src/main/java/gtn/automation/testing/data/dt_FormValidation.xlsx
+++ b/src/main/java/gtn/automation/testing/data/dt_FormValidation.xlsx
@@ -14,16 +14,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>krypton</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pno</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>cmpName</t>
+  </si>
+  <si>
+    <t>add1</t>
+  </si>
+  <si>
+    <t>add2</t>
+  </si>
+  <si>
+    <t>attachFilePath</t>
+  </si>
+  <si>
+    <t>skillCount</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>Srinesh</t>
+  </si>
+  <si>
+    <t>Nisala</t>
+  </si>
+  <si>
+    <t>SrineshNisal@Test.com</t>
+  </si>
+  <si>
+    <t>Virtusa</t>
+  </si>
+  <si>
+    <t>Address one</t>
+  </si>
+  <si>
+    <t>Address two</t>
+  </si>
+  <si>
+    <t>C:\Users\snmuhandiram\Desktop\sample.txt</t>
+  </si>
+  <si>
+    <t>skill one,skill two</t>
+  </si>
+  <si>
+    <t>A777000000</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,13 +103,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,13 +135,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -358,23 +449,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>